<commit_message>
finished PCA and updated readme
</commit_message>
<xml_diff>
--- a/experiments/pca/sample_sentences.xlsx
+++ b/experiments/pca/sample_sentences.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="450">
   <si>
     <t>Han</t>
   </si>
@@ -422,12 +422,6 @@
     <t>Siden har hun jobbet for lillesand blomster</t>
   </si>
   <si>
-    <t>Setniner med gutt</t>
-  </si>
-  <si>
-    <t>Setninger med jente</t>
-  </si>
-  <si>
     <t>Fant gutt (10) i koffert - morsiktet for drap</t>
   </si>
   <si>
@@ -594,9 +588,6 @@
   </si>
   <si>
     <t>Jente (18) ble tatt for promillekjøring</t>
-  </si>
-  <si>
-    <t>En helt spesiell tilfeldighet førte til at hun ble tatt</t>
   </si>
   <si>
     <t>gutt i fare</t>
@@ -1782,10 +1773,10 @@
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -29329,305 +29320,300 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="34" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="B1" s="35" t="s">
-        <v>131</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="38" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" s="39" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="38" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="38" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B7" s="39" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="38" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B8" s="39" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B9" s="39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="38" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B10" s="39" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B11" s="39" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="38" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B12" s="39" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B13" s="39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B14" s="39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B15" s="39" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B16" s="39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="38" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B17" s="39" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="38" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B18" s="39" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="38" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B19" s="39" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B20" s="39" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B21" s="39" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="38" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B23" s="39" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B24" s="39" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="38" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B26" s="39" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="38" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B27" s="39" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="39" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B30" s="39" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="38" t="s">
+    <row r="31">
+      <c r="A31" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="B30" s="39" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="39" t="s">
+      <c r="B31" s="41" t="s">
         <v>189</v>
       </c>
-      <c r="B31" s="39" t="s">
+    </row>
+    <row r="32">
+      <c r="A32" s="36" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="40" t="s">
+      <c r="B32" s="37" t="s">
         <v>191</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="B33" s="37" t="s">
         <v>193</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="36" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" s="37" t="s">
         <v>195</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="B35" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="B35" s="37" t="s">
+    </row>
+    <row r="36">
+      <c r="A36" s="38" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="36" t="s">
+      <c r="B36" s="39" t="s">
         <v>199</v>
       </c>
-      <c r="B36" s="37" t="s">
-        <v>200</v>
-      </c>
     </row>
     <row r="37">
-      <c r="A37" s="38" t="s">
-        <v>201</v>
-      </c>
-      <c r="B37" s="39" t="s">
-        <v>202</v>
-      </c>
+      <c r="B37" s="42"/>
     </row>
     <row r="38">
-      <c r="B38" s="42"/>
+      <c r="B38" s="43"/>
     </row>
     <row r="39">
-      <c r="B39" s="43"/>
+      <c r="B39" s="44"/>
     </row>
     <row r="40">
       <c r="B40" s="44"/>
@@ -29714,10 +29700,10 @@
       <c r="B67" s="44"/>
     </row>
     <row r="68">
-      <c r="B68" s="44"/>
+      <c r="B68" s="45"/>
     </row>
     <row r="69">
-      <c r="B69" s="45"/>
+      <c r="B69" s="43"/>
     </row>
     <row r="70">
       <c r="B70" s="43"/>
@@ -29729,10 +29715,10 @@
       <c r="B72" s="43"/>
     </row>
     <row r="73">
-      <c r="B73" s="43"/>
+      <c r="B73" s="44"/>
     </row>
     <row r="74">
-      <c r="B74" s="44"/>
+      <c r="B74" s="42"/>
     </row>
     <row r="75">
       <c r="B75" s="42"/>
@@ -32487,16 +32473,13 @@
     </row>
     <row r="992">
       <c r="B992" s="42"/>
-    </row>
-    <row r="993">
-      <c r="B993" s="42"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="A2"/>
     <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="A36"/>
-    <hyperlink r:id="rId4" ref="B36"/>
+    <hyperlink r:id="rId3" ref="A35"/>
+    <hyperlink r:id="rId4" ref="B35"/>
   </hyperlinks>
   <drawing r:id="rId5"/>
 </worksheet>
@@ -33038,794 +33021,794 @@
     </row>
     <row r="66">
       <c r="A66" s="47" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B66" s="48" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="47" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B67" s="49" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="47" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B68" s="49" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="47" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B69" s="49" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="47" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B70" s="49" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="50" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B71" s="51" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="47" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B72" s="49" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="47" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B73" s="49" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="47" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B74" s="49" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="47" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B75" s="49" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="47" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B76" s="49" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="47" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B77" s="49" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="47" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B78" s="49" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="52" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B79" s="53" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="47" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B80" s="49" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="47" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B81" s="49" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="47" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B82" s="49" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="47" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B83" s="49" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="47" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B84" s="49" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="47" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B85" s="49" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="50" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B86" s="51" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="47" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B87" s="48" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="47" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B88" s="48" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="47" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B89" s="49" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="47" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B90" s="49" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="47" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B91" s="49" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="54" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B92" s="55" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="47" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B93" s="49" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="52" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B94" s="53" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="47" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B95" s="49" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="52" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B96" s="53" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="52" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B97" s="53" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="52" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B98" s="53" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="52" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B99" s="53" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="54" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B100" s="56" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="52" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B101" s="53" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="52" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B102" s="53" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="54" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B103" s="56" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="54" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B104" s="56" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="52" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B105" s="53" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="52" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B106" s="53" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="52" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B107" s="53" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="52" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B108" s="53" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="54" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="B109" s="56" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="52" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B110" s="53" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="57" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B111" s="58" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="52" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B112" s="53" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="52" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B113" s="53" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="52" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="B114" s="53" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="54" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B115" s="54" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="54" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B116" s="56" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="54" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B117" s="56" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="54" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B118" s="56" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="54" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B119" s="59" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="54" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B120" s="59" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="54" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B121" s="56" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="54" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B122" s="59" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="54" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B123" s="59" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="52" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="B124" s="53" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="54" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B125" s="56" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="54" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B126" s="59" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="47" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B127" s="49" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="54" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B128" s="56" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="54" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B129" s="56" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="54" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B130" s="59" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="60" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="B131" s="61" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="52" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="B132" s="62" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="52" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="B133" s="62" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="52" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B134" s="53" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="52" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B135" s="53" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="52" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B136" s="53" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="52" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B137" s="53" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="52" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B138" s="53" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="52" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B139" s="53" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="52" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B140" s="53" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="52" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B141" s="62" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="47" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B142" s="48" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="47" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="B143" s="49" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="47" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="B144" s="49" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="47" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="B145" s="48" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="52" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="B146" s="53" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="52" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="B147" s="53" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="52" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="B148" s="53" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="52" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="B149" s="53" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="52" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B150" s="53" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="52" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B151" s="53" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="52" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B152" s="53" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="52" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B153" s="53" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="52" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="B154" s="53" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="54" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B155" s="59" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="52" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="B156" s="53" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="52" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="B157" s="62" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="52" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B158" s="53" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="52" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="B159" s="53" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="52" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B160" s="53" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="52" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="B161" s="53" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="52" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B162" s="53" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="52" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="B163" s="53" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="52" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="B164" s="53" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="165">
@@ -37198,7 +37181,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="63" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="B1" s="63" t="s">
         <v>0</v>
@@ -37209,1028 +37192,1028 @@
     </row>
     <row r="2">
       <c r="A2" s="64" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B2" s="65" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C2" s="66" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="64" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="64" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B4" s="65" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="64" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B5" s="65" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="64" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="64" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C7" s="68" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="64" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="64" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C9" s="66" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="64" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="64" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B11" s="65" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C11" s="66" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="64" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C12" s="66" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="64" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B13" s="65" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C13" s="66" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="K13" s="71"/>
     </row>
     <row r="14">
       <c r="A14" s="64" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B14" s="69" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C14" s="70" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="64" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B15" s="72" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="64" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B16" s="69" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C16" s="70" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="74" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B17" s="65" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C17" s="66" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="75"/>
       <c r="B18" s="65" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C18" s="66" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="75"/>
       <c r="B19" s="65" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C19" s="66" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="76" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B20" s="65" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C20" s="66" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="77"/>
       <c r="B21" s="65" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C21" s="66" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="75"/>
       <c r="B22" s="67" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C22" s="68" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="74" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C23" s="66" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="75"/>
       <c r="B24" s="65" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C24" s="66" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="75"/>
       <c r="B25" s="69" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C25" s="70" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="77" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B26" s="65" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C26" s="66" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="75"/>
       <c r="B27" s="65" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C27" s="66" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="75"/>
       <c r="B28" s="78" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C28" s="79" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="77" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B29" s="69" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C29" s="70" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="75"/>
       <c r="B30" s="72" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C30" s="73" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="75"/>
       <c r="B31" s="69" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="C31" s="70" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="77" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B32" s="72" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="C32" s="73" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="75"/>
       <c r="B33" s="72" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C33" s="73" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="75"/>
       <c r="B34" s="72" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="C34" s="73" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="74" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B35" s="72" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C35" s="73" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="75"/>
       <c r="B36" s="80" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C36" s="81" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="75"/>
       <c r="B37" s="72" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C37" s="73" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="74" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B38" s="72" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="C38" s="73" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="75"/>
       <c r="B39" s="78" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C39" s="79" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="75"/>
       <c r="B40" s="78" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C40" s="79" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="64" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B41" s="72" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C41" s="73" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="82" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B42" s="72" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C42" s="73" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="82" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B43" s="72" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C43" s="73" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="82" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B44" s="72" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C44" s="73" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="82" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B45" s="78" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C45" s="79" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="82" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B46" s="72" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C46" s="73" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="82" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B47" s="83" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C47" s="84" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="82" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B48" s="72" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C48" s="73" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="82" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B49" s="72" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C49" s="73" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="82" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B50" s="72" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C50" s="73" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="78" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B51" s="78" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C51" s="85" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="64" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="B52" s="78" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C52" s="79" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="64" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B53" s="78" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C53" s="79" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="64" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B54" s="78" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C54" s="79" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="64" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="B55" s="78" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C55" s="86" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="64" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="B56" s="87" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C56" s="88" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="64" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="B57" s="78" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C57" s="79" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="64" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="B58" s="78" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C58" s="86" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="64" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B59" s="78" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C59" s="86" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="64" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B60" s="72" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C60" s="73" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="64" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="B61" s="78" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C61" s="79" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="64" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="B62" s="87" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C62" s="88" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="64" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B63" s="69" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C63" s="70" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="64" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B64" s="78" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C64" s="79" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="64" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B65" s="78" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C65" s="79" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="64" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B66" s="87" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C66" s="88" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="74" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B67" s="89" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C67" s="90" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="75"/>
       <c r="B68" s="72" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C68" s="73" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="75"/>
       <c r="B69" s="72" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C69" s="73" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="76" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B70" s="72" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C70" s="73" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="77"/>
       <c r="B71" s="72" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C71" s="73" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="75"/>
       <c r="B72" s="72" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C72" s="73" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="74" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B73" s="72" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C73" s="73" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="75"/>
       <c r="B74" s="72" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C74" s="73" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="75"/>
       <c r="B75" s="72" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C75" s="73" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="77" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="B76" s="72" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C76" s="73" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="75"/>
       <c r="B77" s="72" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C77" s="73" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="75"/>
       <c r="B78" s="69" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C78" s="70" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="77" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B79" s="65" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C79" s="66" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="75"/>
       <c r="B80" s="65" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C80" s="66" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="75"/>
       <c r="B81" s="69" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C81" s="70" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="77" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="B82" s="72" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C82" s="73" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="75"/>
       <c r="B83" s="72" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C83" s="73" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="75"/>
       <c r="B84" s="72" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="C84" s="73" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="74" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B85" s="72" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C85" s="73" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="75"/>
       <c r="B86" s="72" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="C86" s="73" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="75"/>
       <c r="B87" s="72" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="C87" s="73" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="74" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B88" s="72" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="C88" s="73" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="75"/>
       <c r="B89" s="72" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="C89" s="73" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="75"/>
       <c r="B90" s="72" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C90" s="73" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="64" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B91" s="78" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C91" s="86" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="82" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="B92" s="72" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C92" s="73" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="82" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B93" s="72" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C93" s="73" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="82" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="B94" s="72" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C94" s="73" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="82" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="B95" s="72" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C95" s="73" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="82" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="B96" s="72" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C96" s="73" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="82" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B97" s="72" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C97" s="73" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="82" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B98" s="72" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C98" s="73" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="82" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="B99" s="72" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C99" s="73" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="82" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="B100" s="72" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C100" s="73" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="101">

</xml_diff>